<commit_message>
added modules pictures; fixed typo in BOM
</commit_message>
<xml_diff>
--- a/BassFly_uHat.bom-varA.xlsx
+++ b/BassFly_uHat.bom-varA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tfa98xx_bt_spkr\kicad5_workspace\projects\BassFly_uHat_Rev1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\bassfly-uhat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59B17E90-7E48-4443-813F-50DAEF799434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDB4EED-626C-4F30-9409-7A72E2D41207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BassFly_uHat.bom" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1211,11 +1211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,10 +1509,10 @@
         <v>110</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>49</v>
@@ -1712,14 +1712,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
-    <hyperlink ref="G7" r:id="rId3"/>
-    <hyperlink ref="G13" r:id="rId4"/>
-    <hyperlink ref="G14" r:id="rId5"/>
-    <hyperlink ref="G15" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
fixed 0.1mm misalignment of mounting holes
</commit_message>
<xml_diff>
--- a/BassFly_uHat.bom-varA.xlsx
+++ b/BassFly_uHat.bom-varA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\bassfly-uhat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tfa98xx_bt_spkr\kicad5_workspace\projects\BassFly_uHat_Rev1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDB4EED-626C-4F30-9409-7A72E2D41207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59B17E90-7E48-4443-813F-50DAEF799434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="BassFly_uHat.bom" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1211,11 +1211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,10 +1509,10 @@
         <v>110</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>49</v>
@@ -1712,14 +1712,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="G13" r:id="rId4"/>
+    <hyperlink ref="G14" r:id="rId5"/>
+    <hyperlink ref="G15" r:id="rId6"/>
+    <hyperlink ref="G10" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>